<commit_message>
add annotation type to comments
</commit_message>
<xml_diff>
--- a/assays/AnnotationContainerAssay/isa.datamap.xlsx
+++ b/assays/AnnotationContainerAssay/isa.datamap.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="isa_datamap" sheetId="1" r:id="R7812bab56f1448ad"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="isa_datamap" sheetId="1" r:id="R671caf969ec74221"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="datamapTable" ref="A1:P5">
-  <x:autoFilter ref="A1:P5"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="datamapTable" ref="A1:Q5">
+  <x:autoFilter ref="A1:Q5"/>
   <x:tableColumns>
     <x:tableColumn id="1" name="Data"/>
     <x:tableColumn id="2" name="Data Format"/>
@@ -26,7 +26,8 @@
     <x:tableColumn id="13" name="Description"/>
     <x:tableColumn id="14" name="Generated By"/>
     <x:tableColumn id="15" name="organism"/>
-    <x:tableColumn id="16" name="file type"/>
+    <x:tableColumn id="16" name="annotation type"/>
+    <x:tableColumn id="17" name="file type"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -35,7 +36,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetData>
-    <x:row r="1" spans="1:16">
+    <x:row r="1" spans="1:17">
       <x:c r="A1" t="str">
         <x:v>Data</x:v>
       </x:c>
@@ -82,10 +83,13 @@
         <x:v>organism</x:v>
       </x:c>
       <x:c r="P1" t="str">
+        <x:v>annotation type</x:v>
+      </x:c>
+      <x:c r="Q1" t="str">
         <x:v>file type</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:16">
+    <x:row r="2" spans="1:17">
       <x:c r="A2" t="str">
         <x:v>./assays/AnnotationContainerAssay/dataset/Chlamydomonas\AnnotationFiles\GO.tsv#col=1</x:v>
       </x:c>
@@ -132,10 +136,13 @@
         <x:v>Chlamydomonas</x:v>
       </x:c>
       <x:c r="P2" t="str">
+        <x:v>GO</x:v>
+      </x:c>
+      <x:c r="Q2" t="str">
         <x:v>Annotation file</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:16">
+    <x:row r="3" spans="1:17">
       <x:c r="A3" t="str">
         <x:v>./assays/AnnotationContainerAssay/dataset/Chlamydomonas\AnnotationFiles\Localization.tsv#col=1</x:v>
       </x:c>
@@ -182,10 +189,13 @@
         <x:v>Chlamydomonas</x:v>
       </x:c>
       <x:c r="P3" t="str">
+        <x:v>Localization</x:v>
+      </x:c>
+      <x:c r="Q3" t="str">
         <x:v>Annotation file</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:16">
+    <x:row r="4" spans="1:17">
       <x:c r="A4" t="str">
         <x:v>./assays/AnnotationContainerAssay/dataset/Chlamydomonas\AnnotationFiles\MapMan.tsv#col=1</x:v>
       </x:c>
@@ -232,10 +242,13 @@
         <x:v>Chlamydomonas</x:v>
       </x:c>
       <x:c r="P4" t="str">
+        <x:v>MapMan</x:v>
+      </x:c>
+      <x:c r="Q4" t="str">
         <x:v>Annotation file</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:16">
+    <x:row r="5" spans="1:17">
       <x:c r="A5" t="str">
         <x:v>./assays/AnnotationContainerAssay/dataset/Chlamydomonas\AnnotationFiles\Synonym.tsv#col=1</x:v>
       </x:c>
@@ -282,6 +295,9 @@
         <x:v>Chlamydomonas</x:v>
       </x:c>
       <x:c r="P5" t="str">
+        <x:v>Synonym</x:v>
+      </x:c>
+      <x:c r="Q5" t="str">
         <x:v>Annotation file</x:v>
       </x:c>
     </x:row>

</xml_diff>